<commit_message>
labeled precinct column to match openelex name
</commit_message>
<xml_diff>
--- a/NY_Tioga/Tioga_NY_cleaned.xlsx
+++ b/NY_Tioga/Tioga_NY_cleaned.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITREPOS\gh_kessler\openelections_work\NY_Tioga\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3407E968-A40F-49C8-A5B9-AB5402DE6AF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ADCD9B8-4922-4C71-AAAD-47DCE2381CF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1240" yWindow="810" windowWidth="29040" windowHeight="19780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1240" yWindow="810" windowWidth="29040" windowHeight="19780" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1796,9 +1796,6 @@
     <t>Tom Reed - IND</t>
   </si>
   <si>
-    <t>Election_District</t>
-  </si>
-  <si>
     <t>Frederick J. Akshar II - REP</t>
   </si>
   <si>
@@ -1821,6 +1818,9 @@
   </si>
   <si>
     <t>Christopher S. Friend - IND</t>
+  </si>
+  <si>
+    <t>precinct</t>
   </si>
 </sst>
 </file>
@@ -2262,7 +2262,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:N346"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
+    <sheetView topLeftCell="A104" workbookViewId="0">
       <selection activeCell="A154" sqref="A154"/>
     </sheetView>
   </sheetViews>
@@ -11817,9 +11817,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -11829,7 +11827,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>590</v>
+        <v>598</v>
       </c>
       <c r="B1" t="s">
         <v>575</v>
@@ -13326,7 +13324,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>590</v>
+        <v>598</v>
       </c>
       <c r="B1" t="s">
         <v>584</v>
@@ -14358,7 +14356,7 @@
   <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -14375,19 +14373,19 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>598</v>
+      </c>
+      <c r="B1" t="s">
         <v>590</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>591</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>593</v>
+      </c>
+      <c r="E1" t="s">
         <v>592</v>
-      </c>
-      <c r="D1" t="s">
-        <v>594</v>
-      </c>
-      <c r="E1" t="s">
-        <v>593</v>
       </c>
       <c r="F1" t="s">
         <v>45</v>
@@ -15474,7 +15472,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B7E95C7-A34E-4122-9771-F04CFF50800C}">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -15482,19 +15480,19 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>590</v>
+        <v>598</v>
       </c>
       <c r="B1" t="s">
+        <v>594</v>
+      </c>
+      <c r="C1" t="s">
         <v>595</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>596</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>597</v>
-      </c>
-      <c r="E1" t="s">
-        <v>598</v>
       </c>
       <c r="F1" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
removed dash from write-in col name
</commit_message>
<xml_diff>
--- a/NY_Tioga/Tioga_NY_cleaned.xlsx
+++ b/NY_Tioga/Tioga_NY_cleaned.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITREPOS\gh_kessler\openelections_work\NY_Tioga\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ADCD9B8-4922-4C71-AAAD-47DCE2381CF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C11C1B3-D802-4092-AC2E-9FB9036C98BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1240" yWindow="810" windowWidth="29040" windowHeight="19780" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1240" yWindow="810" windowWidth="29040" windowHeight="19780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="599">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="600">
   <si>
     <t>OFFICIAL RESULTS</t>
   </si>
@@ -1821,6 +1821,9 @@
   </si>
   <si>
     <t>precinct</t>
+  </si>
+  <si>
+    <t>WriteIn</t>
   </si>
 </sst>
 </file>
@@ -11817,7 +11820,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -11851,7 +11856,7 @@
         <v>581</v>
       </c>
       <c r="I1" t="s">
-        <v>45</v>
+        <v>599</v>
       </c>
       <c r="J1" t="s">
         <v>582</v>
@@ -13305,7 +13310,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -13345,7 +13350,7 @@
         <v>589</v>
       </c>
       <c r="H1" t="s">
-        <v>45</v>
+        <v>599</v>
       </c>
       <c r="I1" t="s">
         <v>582</v>
@@ -14356,7 +14361,7 @@
   <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -14388,7 +14393,7 @@
         <v>592</v>
       </c>
       <c r="F1" t="s">
-        <v>45</v>
+        <v>599</v>
       </c>
       <c r="G1" t="s">
         <v>582</v>
@@ -15472,8 +15477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B7E95C7-A34E-4122-9771-F04CFF50800C}">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -15495,7 +15500,7 @@
         <v>597</v>
       </c>
       <c r="F1" t="s">
-        <v>45</v>
+        <v>599</v>
       </c>
       <c r="G1" t="s">
         <v>582</v>

</xml_diff>